<commit_message>
editor submit event making
Former-commit-id: 91dc96d1cb699a5b6c80c4f4d5821e0d9037f989
</commit_message>
<xml_diff>
--- a/document/5 Design DB/자료/foreditordb.xlsx
+++ b/document/5 Design DB/자료/foreditordb.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Editor database attribute</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -130,6 +130,90 @@
   </si>
   <si>
     <t>comments data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>need ajax</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>php insert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>file upload</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>preview upload</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>thumbnail upload</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>file info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user name(author)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>contents subject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>selected tags</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>selected categories</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CC(?)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>once inquiry (db)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>db table list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>communication method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ssaru's works</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>contents article</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.zepp's works
+reference editor.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reference editor php files
+form and annotate
+it's submit to test.php file
+(./php/editor/test.php)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -137,7 +221,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,8 +254,26 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,8 +316,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -223,11 +355,143 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -238,19 +502,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -554,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -566,18 +896,23 @@
     <col min="2" max="2" width="17.875" customWidth="1"/>
     <col min="3" max="3" width="19.75" customWidth="1"/>
     <col min="4" max="4" width="29.75" customWidth="1"/>
+    <col min="5" max="5" width="16.875" customWidth="1"/>
+    <col min="6" max="6" width="20.625" customWidth="1"/>
+    <col min="7" max="7" width="24.125" customWidth="1"/>
+    <col min="8" max="8" width="19.875" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:14" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="18"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -586,22 +921,18 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+    <row r="2" spans="1:14" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -610,22 +941,28 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+    <row r="3" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -635,21 +972,27 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="A4" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>37</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -659,21 +1002,25 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="A5" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="23"/>
+      <c r="G5" s="24" t="s">
+        <v>46</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -683,21 +1030,25 @@
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="A6" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="23"/>
+      <c r="G6" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -707,19 +1058,25 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="A7" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="23"/>
+      <c r="G7" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -729,16 +1086,23 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="A8" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="22"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="8" t="s">
+        <v>40</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -748,17 +1112,19 @@
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="A9" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -767,16 +1133,20 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+    <row r="10" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="27"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="26" t="s">
+        <v>41</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -785,14 +1155,16 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+    <row r="11" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="27"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -801,9 +1173,27 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
     </row>
+    <row r="12" spans="1:14" ht="66" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:G2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>